<commit_message>
manage order BOL update for staging
</commit_message>
<xml_diff>
--- a/testdata/FCfiles/stg/CustomOrder/QA_538.xlsx
+++ b/testdata/FCfiles/stg/CustomOrder/QA_538.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="73">
   <si>
     <t>serviceLevel</t>
   </si>
@@ -238,6 +238,9 @@
   </si>
   <si>
     <t>59071673</t>
+  </si>
+  <si>
+    <t>59072481</t>
   </si>
 </sst>
 </file>
@@ -260,7 +263,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -342,8 +345,18 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -464,11 +477,18 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" borderId="2" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
@@ -482,7 +502,8 @@
     <xf applyBorder="true" applyFill="true" borderId="9" fillId="10" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="11" fillId="12" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="13" fillId="14" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="15" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="16" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="17" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -1084,8 +1105,8 @@
       <c r="P3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Q3" s="10" t="s">
-        <v>69</v>
+      <c r="Q3" s="14" t="s">
+        <v>72</v>
       </c>
       <c r="R3" s="11" t="s">
         <v>70</v>

</xml_diff>